<commit_message>
final version of wiego paper
</commit_message>
<xml_diff>
--- a/Tables/paneliv_sp.xlsx
+++ b/Tables/paneliv_sp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Statistics\P27\IMSS\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504DA39C-C1BF-400D-AFEB-608A67454BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2038932-2FDC-4A54-B06D-94539C56AE03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7110" yWindow="4380" windowWidth="21600" windowHeight="11175" xr2:uid="{754054C7-3ED2-47E5-9AEC-F82ED7E47689}"/>
+    <workbookView xWindow="19090" yWindow="1800" windowWidth="19420" windowHeight="11500" xr2:uid="{754054C7-3ED2-47E5-9AEC-F82ED7E47689}"/>
   </bookViews>
   <sheets>
     <sheet name="paneliv_sp" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>Number of municipalities</t>
   </si>
@@ -58,15 +58,6 @@
     <t>\checkmark</t>
   </si>
   <si>
-    <t>All</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>DepVarMean</t>
-  </si>
-  <si>
     <t>Employers</t>
   </si>
   <si>
@@ -77,15 +68,6 @@
   </si>
   <si>
     <t>Employment</t>
-  </si>
-  <si>
-    <t>(1)</t>
-  </si>
-  <si>
-    <t>(2)</t>
-  </si>
-  <si>
-    <t>Wages</t>
   </si>
 </sst>
 </file>
@@ -109,7 +91,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -124,17 +106,6 @@
         <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -161,15 +132,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -179,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -187,27 +149,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -259,12 +211,6 @@
           <cell r="D5" t="str">
             <v>-0.0031</v>
           </cell>
-          <cell r="E5" t="str">
-            <v>0.022</v>
-          </cell>
-          <cell r="F5" t="str">
-            <v>-0.016*</v>
-          </cell>
         </row>
         <row r="6">
           <cell r="A6" t="str">
@@ -279,12 +225,6 @@
           <cell r="D6" t="str">
             <v>(0.0067)</v>
           </cell>
-          <cell r="E6" t="str">
-            <v>(0.019)</v>
-          </cell>
-          <cell r="F6" t="str">
-            <v>(0.0085)</v>
-          </cell>
         </row>
         <row r="23">
           <cell r="B23" t="str">
@@ -296,12 +236,6 @@
           <cell r="D23" t="str">
             <v>30331</v>
           </cell>
-          <cell r="E23" t="str">
-            <v>30714</v>
-          </cell>
-          <cell r="F23" t="str">
-            <v>30714</v>
-          </cell>
         </row>
         <row r="25">
           <cell r="A25" t="str">
@@ -316,12 +250,6 @@
           <cell r="D25" t="str">
             <v>6.05</v>
           </cell>
-          <cell r="E25" t="str">
-            <v>5.61</v>
-          </cell>
-          <cell r="F25" t="str">
-            <v>4.04</v>
-          </cell>
         </row>
         <row r="26">
           <cell r="B26" t="str">
@@ -332,12 +260,6 @@
           </cell>
           <cell r="D26" t="str">
             <v>1626</v>
-          </cell>
-          <cell r="E26" t="str">
-            <v>1642</v>
-          </cell>
-          <cell r="F26" t="str">
-            <v>1642</v>
           </cell>
         </row>
       </sheetData>
@@ -643,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE83B80B-01FE-4FF0-8625-92A702BBA6D0}">
-  <dimension ref="A2:O26"/>
+  <dimension ref="A2:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,38 +581,38 @@
   <sheetData>
     <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
-      <c r="B2" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
+      <c r="B2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>11</v>
+      <c r="A3" s="7"/>
+      <c r="B3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="str">
+      <c r="A4" s="3" t="str">
         <f>[1]paneliv_sp!A2</f>
         <v/>
       </c>
-      <c r="B4" s="8" t="str">
+      <c r="B4" s="6" t="str">
         <f>[1]paneliv_sp!B2</f>
         <v>(1)</v>
       </c>
-      <c r="C4" s="8" t="str">
+      <c r="C4" s="6" t="str">
         <f>[1]paneliv_sp!C2</f>
         <v>(2)</v>
       </c>
-      <c r="D4" s="8" t="str">
+      <c r="D4" s="6" t="str">
         <f>[1]paneliv_sp!D2</f>
         <v>(3)</v>
       </c>
@@ -733,18 +655,18 @@
       <c r="O6" s="1"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="7" t="str">
+      <c r="B8" s="5" t="str">
         <f>[1]paneliv_sp!B23</f>
         <v>30331</v>
       </c>
-      <c r="C8" s="7" t="str">
+      <c r="C8" s="5" t="str">
         <f>[1]paneliv_sp!C23</f>
         <v>30331</v>
       </c>
-      <c r="D8" s="7" t="str">
+      <c r="D8" s="5" t="str">
         <f>[1]paneliv_sp!D23</f>
         <v>30331</v>
       </c>
@@ -799,185 +721,23 @@
       </c>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="15"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-    </row>
-    <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="15"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="1" t="str">
-        <f>[1]paneliv_sp!E5</f>
-        <v>0.022</v>
-      </c>
-      <c r="C17" s="1" t="str">
-        <f>[1]paneliv_sp!F5</f>
-        <v>-0.016*</v>
-      </c>
-      <c r="D17" s="15"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="1" t="str">
-        <f>[1]paneliv_sp!E6</f>
-        <v>(0.019)</v>
-      </c>
-      <c r="C18" s="1" t="str">
-        <f>[1]paneliv_sp!F6</f>
-        <v>(0.0085)</v>
-      </c>
-      <c r="D18" s="15"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19"/>
-      <c r="C19"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="7" t="str">
-        <f>[1]paneliv_sp!E23</f>
-        <v>30714</v>
-      </c>
-      <c r="C20" s="7" t="str">
-        <f>[1]paneliv_sp!F23</f>
-        <v>30714</v>
-      </c>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="14"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="1" t="str">
-        <f>[1]paneliv_sp!E26</f>
-        <v>1642</v>
-      </c>
-      <c r="C21" s="1" t="str">
-        <f>[1]paneliv_sp!F26</f>
-        <v>1642</v>
-      </c>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="14"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="1" t="str">
-        <f>[1]paneliv_sp!E25</f>
-        <v>5.61</v>
-      </c>
-      <c r="C22" s="1" t="str">
-        <f>[1]paneliv_sp!F25</f>
-        <v>4.04</v>
-      </c>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="14"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="15"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="15"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D25" s="15"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D26" s="15"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B14:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>